<commit_message>
Adapt repeatable metadata in XLSX file dictionaries
</commit_message>
<xml_diff>
--- a/opal-import/dictionaries/vhf.analysis_nt_pro_bnp-dictionary.xlsx
+++ b/opal-import/dictionaries/vhf.analysis_nt_pro_bnp-dictionary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="45">
   <si>
     <t xml:space="preserve">table</t>
   </si>
@@ -71,9 +71,6 @@
     <t xml:space="preserve">Extension</t>
   </si>
   <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
     <t xml:space="preserve">encounter.id</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">Stroke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
   </si>
   <si>
     <t xml:space="preserve">pid</t>
@@ -170,6 +170,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -266,13 +267,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -322,20 +323,20 @@
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>18</v>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,25 +344,25 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="0" t="n">
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>18</v>
+      <c r="K3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,25 +370,25 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>18</v>
+      <c r="L4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,25 +396,25 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="0" t="n">
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="K5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>18</v>
+      <c r="K5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,25 +422,25 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>18</v>
+      <c r="K6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -447,25 +448,25 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="K7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>18</v>
+      <c r="K7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,25 +474,25 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>18</v>
+      <c r="L8" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,25 +500,25 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>18</v>
+      <c r="L9" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,25 +526,25 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>18</v>
+      <c r="L10" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,25 +552,25 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="K11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>18</v>
+      <c r="K11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,25 +578,25 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="K12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>18</v>
+      <c r="K12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,25 +604,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,25 +630,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="K14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>18</v>
+      <c r="K14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -655,51 +656,77 @@
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="0" t="s">
+      <c r="C16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="J15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L16" s="0" t="s">
-        <v>18</v>
+      <c r="L17" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -724,7 +751,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>